<commit_message>
commit 3 rama 2 para el reto
</commit_message>
<xml_diff>
--- a/datos/Data.xlsx
+++ b/datos/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Search</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>KOORUI Monitor de computadora de 27 pulgadas, QHD 2560P Monitor para juegos de 144 Hz (1 ms, panel VA curvado 1800R, DP1.2+HDMI*2, AdaptiveSync, bisel estrecho con ultrafino), inclinación ajustable, cuidado de los ojos</t>
+  </si>
+  <si>
+    <t>SANSUI Monitor de computadora 24 pulgadas IPS pantalla 75Hz FHD 1080P Monitor de PC 2.953 x 2.953 in VESA con HDMI, puertos VGA sin marco, cuidado de los ojos/altavoces duales para oficina y hogar (ES-24X5AL)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>